<commit_message>
Ready to submit: HF1
</commit_message>
<xml_diff>
--- a/HF1/WP871Q-ExcelSolver.xlsx
+++ b/HF1/WP871Q-ExcelSolver.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kissdanielmark/Library/Mobile Documents/com~apple~CloudDocs/Documents/01.Iskola/BME/MSc - I/02.Operációkutatás/Házi feladat/Házi feladat 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kissdanielmark/Documents/01.Iskola/MSc/1/Operaciokutatas/HF/Operaciokutatas/HF1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2086B0CB-E715-4F40-8AFB-DCEB47B5D6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E984087D-F637-CA4D-B660-793F7BBF62D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25500" windowHeight="19100" xr2:uid="{4BEDAFA8-8981-6148-B186-8DF22C52DE08}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16800" windowHeight="19160" xr2:uid="{4BEDAFA8-8981-6148-B186-8DF22C52DE08}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
+    <sheet name="Eredményjelentés 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Érzékenységi jelentés 1" sheetId="3" r:id="rId3"/>
+    <sheet name="Korlátjelentés 1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Munka1!$C$5:$E$5</definedName>
@@ -85,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="86">
   <si>
     <t>Változók</t>
   </si>
@@ -154,12 +157,213 @@
   <si>
     <t>Az utolsó raktár kapacitását kell növelni, mert az idő ilyen szempontból nem számít, vagyis annyiban hogy max 800kg-ot lehet onnen felvenni 40 perc alatt</t>
   </si>
+  <si>
+    <t>Microsoft Excel 16.73 Eredményjelentés</t>
+  </si>
+  <si>
+    <t>Munkalap: [WP871Q-ExcelSolver.xlsx]Munka1</t>
+  </si>
+  <si>
+    <t>Készült: 2023. 06. 01. 11:39:01</t>
+  </si>
+  <si>
+    <t>Eredmény: A Solver megoldást talált. Az összes korlátozó és optimalizálási feltétel teljesült.</t>
+  </si>
+  <si>
+    <t>Solver motor</t>
+  </si>
+  <si>
+    <t>Motor: Szimplex LP</t>
+  </si>
+  <si>
+    <t>Megoldási idő: 1058,44 másodperc.</t>
+  </si>
+  <si>
+    <t>Közelítő lépések: 5 Részproblémák: 0</t>
+  </si>
+  <si>
+    <t>A Solver beállításai</t>
+  </si>
+  <si>
+    <t>Maximális idő Korlátlan, Iterations Korlátlan, Precision 0,000001</t>
+  </si>
+  <si>
+    <t>Részproblémák maximális száma Korlátlan, Egész megoldások maximális száma Korlátlan, Egész megoldások tűrése 1%, Megoldás egész értékű korlátozó feltételek nélkül, Nemnegatív feltételezése</t>
+  </si>
+  <si>
+    <t>Célértékcella (Min)</t>
+  </si>
+  <si>
+    <t>Cella</t>
+  </si>
+  <si>
+    <t>Név</t>
+  </si>
+  <si>
+    <t>Eredeti érték</t>
+  </si>
+  <si>
+    <t>Végérték</t>
+  </si>
+  <si>
+    <t>Változócellák</t>
+  </si>
+  <si>
+    <t>Egész</t>
+  </si>
+  <si>
+    <t>Korlátozó feltételek</t>
+  </si>
+  <si>
+    <t>Cellaérték</t>
+  </si>
+  <si>
+    <t>Képlet</t>
+  </si>
+  <si>
+    <t>Állapot</t>
+  </si>
+  <si>
+    <t>Korlátváltozó</t>
+  </si>
+  <si>
+    <t>$G$16</t>
+  </si>
+  <si>
+    <t>$C$5</t>
+  </si>
+  <si>
+    <t>Üzem Raktár 1</t>
+  </si>
+  <si>
+    <t>Folytonos</t>
+  </si>
+  <si>
+    <t>$D$5</t>
+  </si>
+  <si>
+    <t>Üzem Raktár 2</t>
+  </si>
+  <si>
+    <t>$E$5</t>
+  </si>
+  <si>
+    <t>Üzem Raktár 3</t>
+  </si>
+  <si>
+    <t>$C$14</t>
+  </si>
+  <si>
+    <t>Maximum ennyit tudnak felpakolni 40 p alatt &lt;=</t>
+  </si>
+  <si>
+    <t>$C$14&gt;=$C$5</t>
+  </si>
+  <si>
+    <t>Nem korlátoz</t>
+  </si>
+  <si>
+    <t>$D$14</t>
+  </si>
+  <si>
+    <t>$D$14&gt;=$D$5</t>
+  </si>
+  <si>
+    <t>$E$14</t>
+  </si>
+  <si>
+    <t>$E$14&gt;=$E$5</t>
+  </si>
+  <si>
+    <t>$F$5</t>
+  </si>
+  <si>
+    <t>$F$5=$H$5</t>
+  </si>
+  <si>
+    <t>Korlátoz</t>
+  </si>
+  <si>
+    <t>$C$5&lt;=$C$7</t>
+  </si>
+  <si>
+    <t>$D$5&lt;=$D$7</t>
+  </si>
+  <si>
+    <t>$E$5&lt;=$E$7</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.73 Érzékenységi jelentés</t>
+  </si>
+  <si>
+    <t>Készült: 2023. 06. 01. 11:39:02</t>
+  </si>
+  <si>
+    <t>Végső</t>
+  </si>
+  <si>
+    <t>Érték</t>
+  </si>
+  <si>
+    <t>Csökkentett</t>
+  </si>
+  <si>
+    <t>költség</t>
+  </si>
+  <si>
+    <t>Célérték</t>
+  </si>
+  <si>
+    <t>együtthatója</t>
+  </si>
+  <si>
+    <t>Megengedhető</t>
+  </si>
+  <si>
+    <t>Növelés</t>
+  </si>
+  <si>
+    <t>Csökkentés</t>
+  </si>
+  <si>
+    <t>Árnyék</t>
+  </si>
+  <si>
+    <t>ár</t>
+  </si>
+  <si>
+    <t>Korlátozó feltétel</t>
+  </si>
+  <si>
+    <t>jobb oldal</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.73 Korlátjelentés</t>
+  </si>
+  <si>
+    <t>Készült: 2023. 06. 01. 11:39:03</t>
+  </si>
+  <si>
+    <t>Változó</t>
+  </si>
+  <si>
+    <t>Alsó</t>
+  </si>
+  <si>
+    <t>korlát</t>
+  </si>
+  <si>
+    <t>Eredmény</t>
+  </si>
+  <si>
+    <t>Felső</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -189,6 +393,23 @@
       <name val="Calibri (Szövegtörzs)"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -216,7 +437,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -342,11 +563,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -361,6 +631,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -677,12 +961,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148BB70A-04F5-2F4D-871E-D5FD04CD885B}">
   <dimension ref="B2:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -717,10 +1005,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="4">
-        <v>550</v>
+        <v>600</v>
       </c>
       <c r="E5" s="5">
-        <v>650</v>
+        <v>600</v>
       </c>
       <c r="F5">
         <f>SUM(C5:E5)</f>
@@ -854,7 +1142,7 @@
       </c>
       <c r="G16" s="9">
         <f>SUMPRODUCT(C5:E5,C16:E16)</f>
-        <v>2300</v>
+        <v>2400</v>
       </c>
       <c r="I16" t="s">
         <v>12</v>
@@ -874,4 +1162,833 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA193E9-7A2F-534E-9B49-357678668981}">
+  <dimension ref="A1:G34"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="12"/>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="16">
+        <v>2300</v>
+      </c>
+      <c r="E16" s="16">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="17">
+        <v>0</v>
+      </c>
+      <c r="E21" s="17">
+        <v>0</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="17">
+        <v>550</v>
+      </c>
+      <c r="E22" s="17">
+        <v>600</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="16">
+        <v>650</v>
+      </c>
+      <c r="E23" s="16">
+        <v>600</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="17">
+        <v>4000</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="17">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="17">
+        <v>1000</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="17">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="17">
+        <v>800</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G30" s="17">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="17">
+        <v>1200</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G31" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="17">
+        <v>0</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G32" s="15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="17">
+        <v>600</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G33" s="15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="16">
+        <v>600</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G34" s="13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C89CB47-98D1-524B-B08C-2DD216F2973F}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="15">
+        <v>0</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1</v>
+      </c>
+      <c r="F9" s="15">
+        <v>4</v>
+      </c>
+      <c r="G9" s="15">
+        <v>1E+30</v>
+      </c>
+      <c r="H9" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="15">
+        <v>600</v>
+      </c>
+      <c r="E10" s="15">
+        <v>0</v>
+      </c>
+      <c r="F10" s="15">
+        <v>3</v>
+      </c>
+      <c r="G10" s="15">
+        <v>1</v>
+      </c>
+      <c r="H10" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="13">
+        <v>600</v>
+      </c>
+      <c r="E11" s="13">
+        <v>-2</v>
+      </c>
+      <c r="F11" s="13">
+        <v>1</v>
+      </c>
+      <c r="G11" s="13">
+        <v>2</v>
+      </c>
+      <c r="H11" s="13">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="15">
+        <v>4000</v>
+      </c>
+      <c r="E16" s="15">
+        <v>0</v>
+      </c>
+      <c r="F16" s="15">
+        <v>0</v>
+      </c>
+      <c r="G16" s="15">
+        <v>4000</v>
+      </c>
+      <c r="H16" s="15">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="15">
+        <v>1000</v>
+      </c>
+      <c r="E17" s="15">
+        <v>0</v>
+      </c>
+      <c r="F17" s="15">
+        <v>0</v>
+      </c>
+      <c r="G17" s="15">
+        <v>400</v>
+      </c>
+      <c r="H17" s="15">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="15">
+        <v>800</v>
+      </c>
+      <c r="E18" s="15">
+        <v>0</v>
+      </c>
+      <c r="F18" s="15">
+        <v>0</v>
+      </c>
+      <c r="G18" s="15">
+        <v>200</v>
+      </c>
+      <c r="H18" s="15">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="13">
+        <v>1200</v>
+      </c>
+      <c r="E19" s="13">
+        <v>3</v>
+      </c>
+      <c r="F19" s="13">
+        <v>1200</v>
+      </c>
+      <c r="G19" s="13">
+        <v>200</v>
+      </c>
+      <c r="H19" s="13">
+        <v>600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5C4DF9-9612-F945-B53D-FF6016F6FDD4}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" customWidth="1"/>
+    <col min="9" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="18"/>
+    </row>
+    <row r="7" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="16">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="F11" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="17">
+        <v>0</v>
+      </c>
+      <c r="F13" s="17">
+        <v>0</v>
+      </c>
+      <c r="G13" s="17">
+        <v>85</v>
+      </c>
+      <c r="I13" s="17">
+        <v>250</v>
+      </c>
+      <c r="J13" s="17">
+        <v>18835</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="17">
+        <v>600</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0</v>
+      </c>
+      <c r="G14" s="17">
+        <v>110</v>
+      </c>
+      <c r="I14" s="17">
+        <v>398.5</v>
+      </c>
+      <c r="J14" s="17">
+        <v>20035</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="16">
+        <v>600</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0</v>
+      </c>
+      <c r="G15" s="16">
+        <v>125</v>
+      </c>
+      <c r="I15" s="16">
+        <v>597</v>
+      </c>
+      <c r="J15" s="16">
+        <v>21020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>